<commit_message>
4.24 HOME mix p010305
</commit_message>
<xml_diff>
--- a/mix/FFN.xlsx
+++ b/mix/FFN.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\astrocyte_neuron\mix\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E099885-5C0D-406F-A337-E121A533188C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3672" yWindow="4116" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="p07" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,14 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gamma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,11 +87,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +374,590 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A5:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.16550000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.17630000000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.1845</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.19020000000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.19719999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.2009</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.21560000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <v>0.21629999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.2215</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.22839999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.23150000000000001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.2349</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.23810000000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.2404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.22370000000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.23530000000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.2447</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.24879999999999999</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.25140000000000001</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.255</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.25659999999999999</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.25979999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.23469999999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.2407</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.25259999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.25729999999999997</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.2616</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.26579999999999998</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.26929999999999998</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.27150000000000002</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.27460000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.1799</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.1918</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.2024</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.2109</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.218</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.22509999999999999</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.22689999999999999</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.23469999999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.2389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.2109</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.22720000000000001</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.2349</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.23449999999999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.2442</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.24990000000000001</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.25259999999999999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.25769999999999998</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.26019999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.2291</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.2402</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.249</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.2681</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.27160000000000001</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.27539999999999998</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.27929999999999999</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.24260000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.25359999999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.26429999999999998</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.27260000000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.28489999999999999</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.2903</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.2949</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.29870000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.30259999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.1731</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.21679999999999999</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.23139999999999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.23669999999999999</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.24210000000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.25130000000000002</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.25559999999999999</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.2621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.21959999999999999</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
+        <v>0.2475</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.25629999999999997</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.26129999999999998</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.26829999999999998</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.2732</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.2777</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.28710000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.24179999999999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.2576</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.26910000000000001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.27729999999999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.2863</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.29049999999999998</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.30280000000000001</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.30940000000000001</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.31209999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.25929999999999997</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.28849999999999998</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.29880000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.3075</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.3155</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.31990000000000002</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.3296</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.3347</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.34089999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>